<commit_message>
Don't need to convert with fuhep
</commit_message>
<xml_diff>
--- a/Wood 2017 Human Clint and CLh.xlsx
+++ b/Wood 2017 Human Clint and CLh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\NCCT_ExpoCast\ExpoCast2019\HTTKDataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httkdatatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7239544-6D04-4D1B-A0AC-A4E14249853A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CEC9E3-66D3-4516-94AE-7AD60C5317A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="7410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2155,7 +2158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2253,6 +2256,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2569,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2667,9 +2671,9 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2">
-        <f>K2*J2/120/21.4*1000</f>
-        <v>1.8072429906542058</v>
+      <c r="O2" s="33">
+        <f>K2/120/21.4*1000</f>
+        <v>1.985981308411215</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -2715,9 +2719,9 @@
       <c r="N3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O3">
-        <f>K3*J3/120/21.4*1000</f>
-        <v>1.0140186915887852</v>
+      <c r="O3" s="33">
+        <f t="shared" ref="O3:O66" si="0">K3/120/21.4*1000</f>
+        <v>1.0903426791277258</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -2755,6 +2759,10 @@
       <c r="N4" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="O4" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
@@ -2799,9 +2807,9 @@
       <c r="N5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O5">
-        <f t="shared" ref="O5:O67" si="0">K5*J5/120/21.4*1000</f>
-        <v>0.36214953271028044</v>
+      <c r="O5" s="33">
+        <f t="shared" si="0"/>
+        <v>0.38940809968847356</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2847,9 +2855,9 @@
       <c r="N6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="33">
         <f t="shared" si="0"/>
-        <v>19.528816199376948</v>
+        <v>22.975077881619935</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -2895,9 +2903,9 @@
       <c r="N7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="33">
         <f t="shared" si="0"/>
-        <v>1.8691588785046729</v>
+        <v>12.461059190031154</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2935,6 +2943,10 @@
       <c r="N8" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="O8" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
@@ -2979,9 +2991,9 @@
       <c r="N9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="33">
         <f t="shared" si="0"/>
-        <v>0.48091900311526481</v>
+        <v>0.50623052959501558</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -3027,9 +3039,9 @@
       <c r="N10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="33">
         <f t="shared" si="0"/>
-        <v>1.8866822429906545</v>
+        <v>1.985981308411215</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -3067,6 +3079,10 @@
       <c r="N11" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="O11" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
@@ -3111,9 +3127,9 @@
       <c r="N12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="33">
         <f t="shared" si="0"/>
-        <v>1.6919781931464177</v>
+        <v>2.1417445482866042</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3159,9 +3175,9 @@
       <c r="N13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="33">
         <f t="shared" si="0"/>
-        <v>1.8925233644859814</v>
+        <v>2.3364485981308416</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3207,9 +3223,9 @@
       <c r="N14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="33">
         <f t="shared" si="0"/>
-        <v>7.2819314641744564</v>
+        <v>13.2398753894081</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3255,9 +3271,9 @@
       <c r="N15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="33">
         <f t="shared" si="0"/>
-        <v>10.630841121495326</v>
+        <v>30.373831775700939</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3303,9 +3319,9 @@
       <c r="N16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="33">
         <f t="shared" si="0"/>
-        <v>1.9813084112149533</v>
+        <v>2.0638629283489101</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3345,9 +3361,9 @@
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
-      <c r="O17">
+      <c r="O17" s="33">
         <f t="shared" si="0"/>
-        <v>1.995327102803738</v>
+        <v>2.3753894080996885</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3393,9 +3409,9 @@
       <c r="N18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="33">
         <f t="shared" si="0"/>
-        <v>37.437694704049846</v>
+        <v>98.520249221183818</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3435,9 +3451,9 @@
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
-      <c r="O19">
+      <c r="O19" s="33">
         <f t="shared" si="0"/>
-        <v>1.9018691588785048</v>
+        <v>2.8816199376947043</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -3483,9 +3499,9 @@
       <c r="N20" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="33">
         <f t="shared" si="0"/>
-        <v>13.266355140186919</v>
+        <v>195.09345794392524</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3531,9 +3547,9 @@
       <c r="N21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="33">
         <f t="shared" si="0"/>
-        <v>5.1791277258566977</v>
+        <v>5.4517133956386301</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -3579,9 +3595,9 @@
       <c r="N22" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="33">
         <f t="shared" si="0"/>
-        <v>5.9968847352024923</v>
+        <v>8.5669781931464168</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3621,9 +3637,9 @@
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
-      <c r="O23">
+      <c r="O23" s="33">
         <f t="shared" si="0"/>
-        <v>22.815420560747665</v>
+        <v>24.532710280373834</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3669,9 +3685,9 @@
       <c r="N24" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="33">
         <f t="shared" si="0"/>
-        <v>3.89797507788162</v>
+        <v>5.0623052959501562</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="48" x14ac:dyDescent="0.25">
@@ -3717,9 +3733,9 @@
       <c r="N25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="33">
         <f t="shared" si="0"/>
-        <v>4.7975077881619947</v>
+        <v>29.984423676012465</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3765,9 +3781,9 @@
       <c r="N26" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="33">
         <f t="shared" si="0"/>
-        <v>1.6121495327102802</v>
+        <v>1.7912772585669781</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -3813,9 +3829,9 @@
       <c r="N27" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="33">
         <f t="shared" si="0"/>
-        <v>1.1775700934579441</v>
+        <v>2.1806853582554515</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -3861,9 +3877,9 @@
       <c r="N28" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="33">
         <f t="shared" si="0"/>
-        <v>61.495327102803735</v>
+        <v>65.420560747663544</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3903,9 +3919,9 @@
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
-      <c r="O29">
+      <c r="O29" s="33">
         <f t="shared" si="0"/>
-        <v>2.8855140186915889</v>
+        <v>3.0373831775700939</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -3951,9 +3967,9 @@
       <c r="N30" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="33">
         <f t="shared" si="0"/>
-        <v>4.9065420560747661</v>
+        <v>13.629283489096574</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -3999,9 +4015,9 @@
       <c r="N31" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="33">
         <f t="shared" si="0"/>
-        <v>4.0303738317757007</v>
+        <v>5.8411214953271031</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -4047,9 +4063,9 @@
       <c r="N32" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="33">
         <f t="shared" si="0"/>
-        <v>9.1588785046728969</v>
+        <v>19.080996884735203</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -4087,6 +4103,10 @@
       <c r="N33" s="7" t="s">
         <v>162</v>
       </c>
+      <c r="O33" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:15" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
@@ -4131,9 +4151,9 @@
       <c r="N34" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="33">
         <f t="shared" si="0"/>
-        <v>10.728193146417444</v>
+        <v>11.292834890965734</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4173,9 +4193,9 @@
       <c r="L35" s="14"/>
       <c r="M35" s="14"/>
       <c r="N35" s="14"/>
-      <c r="O35">
+      <c r="O35" s="33">
         <f t="shared" si="0"/>
-        <v>5.8566978193146415</v>
+        <v>6.230529595015577</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -4215,9 +4235,9 @@
       <c r="L36" s="14"/>
       <c r="M36" s="14"/>
       <c r="N36" s="14"/>
-      <c r="O36">
+      <c r="O36" s="33">
         <f t="shared" si="0"/>
-        <v>0.97040498442367606</v>
+        <v>1.0903426791277258</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -4263,9 +4283,9 @@
       <c r="N37" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="33">
         <f t="shared" si="0"/>
-        <v>4.6612149532710285</v>
+        <v>7.3987538940809969</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4303,6 +4323,10 @@
       <c r="N38" s="7" t="s">
         <v>181</v>
       </c>
+      <c r="O38" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
@@ -4347,9 +4371,9 @@
       <c r="N39" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="33">
         <f t="shared" si="0"/>
-        <v>48.528037383177569</v>
+        <v>52.18068535825546</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4395,9 +4419,9 @@
       <c r="N40" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="33">
         <f t="shared" si="0"/>
-        <v>3.4345794392523366</v>
+        <v>3.8161993769470413</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4437,9 +4461,9 @@
       <c r="L41" s="14"/>
       <c r="M41" s="14"/>
       <c r="N41" s="14"/>
-      <c r="O41">
+      <c r="O41" s="33">
         <f t="shared" si="0"/>
-        <v>1.5327102803738317</v>
+        <v>1.5965732087227413</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -4485,9 +4509,9 @@
       <c r="N42" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="33">
         <f t="shared" si="0"/>
-        <v>6.156542056074767</v>
+        <v>6.61993769470405</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -4527,9 +4551,9 @@
       <c r="L43" s="14"/>
       <c r="M43" s="14"/>
       <c r="N43" s="14"/>
-      <c r="O43">
+      <c r="O43" s="33">
         <f t="shared" si="0"/>
-        <v>6.0981308411214954</v>
+        <v>7.009345794392523</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -4569,9 +4593,9 @@
       <c r="L44" s="14"/>
       <c r="M44" s="14"/>
       <c r="N44" s="14"/>
-      <c r="O44">
+      <c r="O44" s="33">
         <f t="shared" si="0"/>
-        <v>2.8348909657320878</v>
+        <v>5.0623052959501562</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -4609,6 +4633,10 @@
       <c r="N45" s="7" t="s">
         <v>213</v>
       </c>
+      <c r="O45" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
@@ -4653,9 +4681,9 @@
       <c r="N46" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="O46">
+      <c r="O46" s="33">
         <f t="shared" si="0"/>
-        <v>7.9672897196261703</v>
+        <v>8.5669781931464168</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -4701,9 +4729,9 @@
       <c r="N47" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="33">
         <f t="shared" si="0"/>
-        <v>9.5171339563862922</v>
+        <v>10.124610591900312</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -4749,9 +4777,9 @@
       <c r="N48" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="33">
         <f t="shared" si="0"/>
-        <v>6.3084112149532707</v>
+        <v>35.046728971962622</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4791,9 +4819,9 @@
       <c r="L49" s="14"/>
       <c r="M49" s="14"/>
       <c r="N49" s="14"/>
-      <c r="O49">
+      <c r="O49" s="33">
         <f t="shared" si="0"/>
-        <v>9.9883177570093462</v>
+        <v>10.514018691588786</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -4833,9 +4861,9 @@
       <c r="L50" s="14"/>
       <c r="M50" s="14"/>
       <c r="N50" s="14"/>
-      <c r="O50">
+      <c r="O50" s="33">
         <f t="shared" si="0"/>
-        <v>12.811526479750778</v>
+        <v>13.629283489096574</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -4875,9 +4903,9 @@
       <c r="L51" s="14"/>
       <c r="M51" s="14"/>
       <c r="N51" s="14"/>
-      <c r="O51">
+      <c r="O51" s="33">
         <f t="shared" si="0"/>
-        <v>46.074766355140191</v>
+        <v>52.9595015576324</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -4923,9 +4951,9 @@
       <c r="N52" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O52">
+      <c r="O52" s="33">
         <f t="shared" si="0"/>
-        <v>4.4859813084112146</v>
+        <v>4.6728971962616832</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4971,9 +4999,9 @@
       <c r="N53" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="O53">
+      <c r="O53" s="33">
         <f t="shared" si="0"/>
-        <v>5.4322429906542062</v>
+        <v>5.8411214953271031</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -5013,9 +5041,9 @@
       <c r="L54" s="14"/>
       <c r="M54" s="14"/>
       <c r="N54" s="14"/>
-      <c r="O54">
+      <c r="O54" s="33">
         <f t="shared" si="0"/>
-        <v>2.004672897196262</v>
+        <v>3.0373831775700939</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5061,9 +5089,9 @@
       <c r="N55" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="O55">
+      <c r="O55" s="33">
         <f t="shared" si="0"/>
-        <v>4.5560747663551409</v>
+        <v>5.0623052959501562</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5109,9 +5137,9 @@
       <c r="N56" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="O56">
+      <c r="O56" s="33">
         <f t="shared" si="0"/>
-        <v>0.62889408099688471</v>
+        <v>0.7398753894080996</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5157,9 +5185,9 @@
       <c r="N57" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="O57">
+      <c r="O57" s="33">
         <f t="shared" si="0"/>
-        <v>5.8917445482866055</v>
+        <v>34.657320872274148</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -5197,6 +5225,10 @@
       <c r="N58" s="7" t="s">
         <v>267</v>
       </c>
+      <c r="O58" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
@@ -5233,6 +5265,10 @@
       <c r="N59" s="7" t="s">
         <v>271</v>
       </c>
+      <c r="O59" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
@@ -5269,6 +5305,10 @@
       <c r="N60" s="7" t="s">
         <v>276</v>
       </c>
+      <c r="O60" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
@@ -5305,6 +5345,10 @@
       <c r="N61" s="7" t="s">
         <v>281</v>
       </c>
+      <c r="O61" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:15" ht="36" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
@@ -5349,9 +5393,9 @@
       <c r="N62" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="O62">
+      <c r="O62" s="33">
         <f t="shared" si="0"/>
-        <v>4.7429906542056068</v>
+        <v>5.4517133956386301</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -5391,9 +5435,9 @@
       <c r="L63" s="14"/>
       <c r="M63" s="14"/>
       <c r="N63" s="14"/>
-      <c r="O63">
+      <c r="O63" s="33">
         <f t="shared" si="0"/>
-        <v>2.1074766355140184</v>
+        <v>2.5700934579439254</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -5439,9 +5483,9 @@
       <c r="N64" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="O64">
+      <c r="O64" s="33">
         <f t="shared" si="0"/>
-        <v>5.6074766355140193</v>
+        <v>6.230529595015577</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -5487,9 +5531,9 @@
       <c r="N65" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="O65">
+      <c r="O65" s="33">
         <f t="shared" si="0"/>
-        <v>4.8481308411214954</v>
+        <v>5.8411214953271031</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -5535,9 +5579,9 @@
       <c r="N66" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="O66">
+      <c r="O66" s="33">
         <f t="shared" si="0"/>
-        <v>15.046728971962619</v>
+        <v>16.355140186915886</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5577,9 +5621,9 @@
       <c r="L67" s="14"/>
       <c r="M67" s="14"/>
       <c r="N67" s="14"/>
-      <c r="O67">
-        <f t="shared" si="0"/>
-        <v>12.133956386292835</v>
+      <c r="O67" s="33">
+        <f t="shared" ref="O67:O119" si="1">K67/120/21.4*1000</f>
+        <v>29.595015576323988</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5625,9 +5669,9 @@
       <c r="N68" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="O68">
-        <f t="shared" ref="O68:O119" si="1">K68*J68/120/21.4*1000</f>
-        <v>3.0015576323987538</v>
+      <c r="O68" s="33">
+        <f t="shared" si="1"/>
+        <v>3.1931464174454827</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -5673,9 +5717,9 @@
       <c r="N69" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="O69">
+      <c r="O69" s="33">
         <f t="shared" si="1"/>
-        <v>60.478971962616832</v>
+        <v>65.031152647975091</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -5715,9 +5759,9 @@
       <c r="L70" s="14"/>
       <c r="M70" s="14"/>
       <c r="N70" s="14"/>
-      <c r="O70">
+      <c r="O70" s="33">
         <f t="shared" si="1"/>
-        <v>16.838006230529594</v>
+        <v>17.912772585669785</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5763,9 +5807,9 @@
       <c r="N71" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="O71">
+      <c r="O71" s="33">
         <f t="shared" si="1"/>
-        <v>24.096573208722749</v>
+        <v>26.4797507788162</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -5811,9 +5855,9 @@
       <c r="N72" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="O72">
+      <c r="O72" s="33">
         <f t="shared" si="1"/>
-        <v>18.45794392523365</v>
+        <v>23.364485981308412</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5851,6 +5895,10 @@
       <c r="N73" s="7" t="s">
         <v>334</v>
       </c>
+      <c r="O73" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
@@ -5889,9 +5937,9 @@
       <c r="L74" s="14"/>
       <c r="M74" s="14"/>
       <c r="N74" s="14"/>
-      <c r="O74">
+      <c r="O74" s="33">
         <f t="shared" si="1"/>
-        <v>7.3637071651090347</v>
+        <v>12.07165109034268</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -5937,9 +5985,9 @@
       <c r="N75" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="O75">
+      <c r="O75" s="33">
         <f t="shared" si="1"/>
-        <v>2.8457943925233646</v>
+        <v>3.2710280373831782</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="48" x14ac:dyDescent="0.25">
@@ -5979,9 +6027,9 @@
       <c r="L76" s="14"/>
       <c r="M76" s="14"/>
       <c r="N76" s="14"/>
-      <c r="O76">
+      <c r="O76" s="33">
         <f t="shared" si="1"/>
-        <v>1.233644859813084</v>
+        <v>1.4018691588785048</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6021,9 +6069,9 @@
       <c r="L77" s="14"/>
       <c r="M77" s="14"/>
       <c r="N77" s="14"/>
-      <c r="O77">
+      <c r="O77" s="33">
         <f t="shared" si="1"/>
-        <v>4.3925233644859816</v>
+        <v>4.6728971962616832</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -6063,9 +6111,9 @@
       <c r="L78" s="14"/>
       <c r="M78" s="14"/>
       <c r="N78" s="14"/>
-      <c r="O78">
+      <c r="O78" s="33">
         <f t="shared" si="1"/>
-        <v>2.8457943925233646</v>
+        <v>3.2710280373831782</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -6105,9 +6153,9 @@
       <c r="L79" s="14"/>
       <c r="M79" s="14"/>
       <c r="N79" s="14"/>
-      <c r="O79">
+      <c r="O79" s="33">
         <f t="shared" si="1"/>
-        <v>3.7694704049844234</v>
+        <v>4.2834890965732084</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -6153,9 +6201,9 @@
       <c r="N80" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="O80">
+      <c r="O80" s="33">
         <f t="shared" si="1"/>
-        <v>8.5046728971962615</v>
+        <v>9.3457943925233664</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -6195,9 +6243,9 @@
       <c r="L81" s="14"/>
       <c r="M81" s="14"/>
       <c r="N81" s="14"/>
-      <c r="O81">
+      <c r="O81" s="33">
         <f t="shared" si="1"/>
-        <v>0.68691588785046731</v>
+        <v>0.81775700934579454</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6237,9 +6285,9 @@
       <c r="L82" s="14"/>
       <c r="M82" s="14"/>
       <c r="N82" s="14"/>
-      <c r="O82">
+      <c r="O82" s="33">
         <f t="shared" si="1"/>
-        <v>2.3033489096573212</v>
+        <v>2.5311526479750781</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="48" x14ac:dyDescent="0.25">
@@ -6285,9 +6333,9 @@
       <c r="N83" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="O83">
+      <c r="O83" s="33">
         <f t="shared" si="1"/>
-        <v>3.14797507788162</v>
+        <v>3.3489096573208728</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -6327,9 +6375,9 @@
       <c r="L84" s="14"/>
       <c r="M84" s="14"/>
       <c r="N84" s="14"/>
-      <c r="O84">
+      <c r="O84" s="33">
         <f t="shared" si="1"/>
-        <v>5.3738317757009346</v>
+        <v>5.8411214953271031</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
@@ -6367,6 +6415,10 @@
       <c r="N85" s="7" t="s">
         <v>383</v>
       </c>
+      <c r="O85" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
@@ -6411,9 +6463,9 @@
       <c r="N86" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="O86">
+      <c r="O86" s="33">
         <f t="shared" si="1"/>
-        <v>4.1433021806853585</v>
+        <v>5.4517133956386301</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -6459,9 +6511,9 @@
       <c r="N87" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="O87">
+      <c r="O87" s="33">
         <f t="shared" si="1"/>
-        <v>5.8722741433021808</v>
+        <v>22.585669781931468</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -6507,9 +6559,9 @@
       <c r="N88" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="O88">
+      <c r="O88" s="33">
         <f t="shared" si="1"/>
-        <v>7.4299065420560737</v>
+        <v>41.277258566978198</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6555,9 +6607,9 @@
       <c r="N89" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="O89">
+      <c r="O89" s="33">
         <f t="shared" si="1"/>
-        <v>19.470404984423677</v>
+        <v>38.940809968847354</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -6603,9 +6655,9 @@
       <c r="N90" s="15" t="s">
         <v>405</v>
       </c>
-      <c r="O90">
+      <c r="O90" s="33">
         <f t="shared" si="1"/>
-        <v>12.266355140186917</v>
+        <v>19.470404984423677</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6651,9 +6703,9 @@
       <c r="N91" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="O91">
+      <c r="O91" s="33">
         <f t="shared" si="1"/>
-        <v>4.6612149532710285</v>
+        <v>7.3987538940809969</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6699,9 +6751,9 @@
       <c r="N92" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="O92">
+      <c r="O92" s="33">
         <f t="shared" si="1"/>
-        <v>5.6425233644859816</v>
+        <v>8.9563862928348925</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -6747,9 +6799,9 @@
       <c r="N93" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="O93">
+      <c r="O93" s="33">
         <f t="shared" si="1"/>
-        <v>4.2367601246105924</v>
+        <v>6.61993769470405</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -6789,9 +6841,9 @@
       <c r="L94" s="14"/>
       <c r="M94" s="14"/>
       <c r="N94" s="14"/>
-      <c r="O94">
+      <c r="O94" s="33">
         <f t="shared" si="1"/>
-        <v>1.2577881619937694</v>
+        <v>1.32398753894081</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -6829,6 +6881,10 @@
       <c r="N95" s="7" t="s">
         <v>426</v>
       </c>
+      <c r="O95" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
@@ -6865,6 +6921,10 @@
       <c r="N96" s="7" t="s">
         <v>430</v>
       </c>
+      <c r="O96" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
@@ -6909,9 +6969,9 @@
       <c r="N97" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="O97">
+      <c r="O97" s="33">
         <f t="shared" si="1"/>
-        <v>8.0685358255451725</v>
+        <v>10.90342679127726</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6951,9 +7011,9 @@
       <c r="L98" s="14"/>
       <c r="M98" s="14"/>
       <c r="N98" s="14"/>
-      <c r="O98">
+      <c r="O98" s="33">
         <f t="shared" si="1"/>
-        <v>3.3411214953271031</v>
+        <v>8.5669781931464168</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -6991,6 +7051,10 @@
       <c r="N99" s="7" t="s">
         <v>442</v>
       </c>
+      <c r="O99" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
@@ -7027,6 +7091,10 @@
       <c r="N100" s="7" t="s">
         <v>446</v>
       </c>
+      <c r="O100" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
@@ -7065,9 +7133,9 @@
       <c r="L101" s="14"/>
       <c r="M101" s="14"/>
       <c r="N101" s="14"/>
-      <c r="O101">
+      <c r="O101" s="33">
         <f t="shared" si="1"/>
-        <v>6.9548286604361369</v>
+        <v>7.3987538940809969</v>
       </c>
     </row>
     <row r="102" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -7113,9 +7181,9 @@
       <c r="N102" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="O102">
+      <c r="O102" s="33">
         <f t="shared" si="1"/>
-        <v>8.5981308411214972</v>
+        <v>9.3457943925233664</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -7155,9 +7223,9 @@
       <c r="L103" s="14"/>
       <c r="M103" s="14"/>
       <c r="N103" s="14"/>
-      <c r="O103">
+      <c r="O103" s="33">
         <f t="shared" si="1"/>
-        <v>2.2694704049844234</v>
+        <v>2.4143302180685362</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -7195,6 +7263,10 @@
       <c r="N104" s="7" t="s">
         <v>461</v>
       </c>
+      <c r="O104" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
@@ -7233,9 +7305,9 @@
       <c r="L105" s="6"/>
       <c r="M105" s="6"/>
       <c r="N105" s="6"/>
-      <c r="O105">
+      <c r="O105" s="33">
         <f t="shared" si="1"/>
-        <v>2.1261682242990654</v>
+        <v>2.3364485981308416</v>
       </c>
     </row>
     <row r="106" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -7281,9 +7353,9 @@
       <c r="N106" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="O106">
+      <c r="O106" s="33">
         <f t="shared" si="1"/>
-        <v>1.794392523364486</v>
+        <v>1.8691588785046729</v>
       </c>
     </row>
     <row r="107" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -7329,9 +7401,9 @@
       <c r="N107" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="O107">
+      <c r="O107" s="33">
         <f t="shared" si="1"/>
-        <v>0.74766355140186924</v>
+        <v>0.77881619937694713</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -7371,9 +7443,9 @@
       <c r="L108" s="14"/>
       <c r="M108" s="14"/>
       <c r="N108" s="14"/>
-      <c r="O108">
+      <c r="O108" s="33">
         <f t="shared" si="1"/>
-        <v>3.4345794392523366</v>
+        <v>3.8161993769470413</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -7419,9 +7491,9 @@
       <c r="N109" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="O109">
+      <c r="O109" s="33">
         <f t="shared" si="1"/>
-        <v>1.0989096573208723</v>
+        <v>1.32398753894081</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -7467,9 +7539,9 @@
       <c r="N110" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="O110">
+      <c r="O110" s="33">
         <f t="shared" si="1"/>
-        <v>6.0669781931464177</v>
+        <v>7.3987538940809969</v>
       </c>
     </row>
     <row r="111" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -7515,9 +7587,9 @@
       <c r="N111" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="O111">
+      <c r="O111" s="33">
         <f t="shared" si="1"/>
-        <v>2.2679127725856705</v>
+        <v>2.4922118380062313</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -7563,9 +7635,9 @@
       <c r="N112" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="O112">
+      <c r="O112" s="33">
         <f t="shared" si="1"/>
-        <v>5.7242990654205617</v>
+        <v>58.411214953271035</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -7611,9 +7683,9 @@
       <c r="N113" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="O113">
+      <c r="O113" s="33">
         <f t="shared" si="1"/>
-        <v>21.464174454828662</v>
+        <v>41.277258566978198</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -7659,9 +7731,9 @@
       <c r="N114" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="O114">
+      <c r="O114" s="33">
         <f t="shared" si="1"/>
-        <v>1.0981308411214954</v>
+        <v>1.1682242990654208</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -7701,9 +7773,9 @@
       <c r="L115" s="14"/>
       <c r="M115" s="14"/>
       <c r="N115" s="14"/>
-      <c r="O115">
+      <c r="O115" s="33">
         <f t="shared" si="1"/>
-        <v>0.98831775700934588</v>
+        <v>1.0514018691588787</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -7743,9 +7815,9 @@
       <c r="L116" s="14"/>
       <c r="M116" s="14"/>
       <c r="N116" s="14"/>
-      <c r="O116">
+      <c r="O116" s="33">
         <f t="shared" si="1"/>
-        <v>2.6152647975077885</v>
+        <v>2.8426791277258565</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -7785,7 +7857,7 @@
       <c r="L117" s="14"/>
       <c r="M117" s="14"/>
       <c r="N117" s="14"/>
-      <c r="O117">
+      <c r="O117" s="33">
         <f t="shared" si="1"/>
         <v>2.4143302180685362</v>
       </c>
@@ -7827,9 +7899,9 @@
       <c r="L118" s="14"/>
       <c r="M118" s="14"/>
       <c r="N118" s="14"/>
-      <c r="O118">
+      <c r="O118" s="33">
         <f t="shared" si="1"/>
-        <v>2.0907320872274147</v>
+        <v>2.2975077881619943</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -7875,9 +7947,9 @@
       <c r="N119" s="11" t="s">
         <v>527</v>
       </c>
-      <c r="O119">
+      <c r="O119" s="33">
         <f t="shared" si="1"/>
-        <v>2.8130841121495331</v>
+        <v>3.2710280373831782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>